<commit_message>
add new countries, add 3 years reference
</commit_message>
<xml_diff>
--- a/Australia/Data/mortality_aus_2015.xlsx
+++ b/Australia/Data/mortality_aus_2015.xlsx
@@ -1,46 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ru48fak\LRZ Sync+Share\Excess Mortality World\Data, Code and Results\Australia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giacomo/Documents/GitHub/excess-mortality-world/Australia/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B9697E-2C40-4342-853E-7C6E1C3EEC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="bltper_1x1" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="life_tables_2015" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="life_tables_new" localSheetId="0">Sheet1!#REF!</definedName>
-    <definedName name="mortality_2015" localSheetId="0">Sheet1!#REF!</definedName>
-    <definedName name="table_2015" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="201">
   <si>
     <t>0</t>
   </si>
@@ -349,12 +339,306 @@
   </si>
   <si>
     <t>110+</t>
+  </si>
+  <si>
+    <t>0.00355</t>
+  </si>
+  <si>
+    <t>0.00131</t>
+  </si>
+  <si>
+    <t>0.00409</t>
+  </si>
+  <si>
+    <t>0.01088</t>
+  </si>
+  <si>
+    <t>0.01429</t>
+  </si>
+  <si>
+    <t>0.00105</t>
+  </si>
+  <si>
+    <t>0.00463</t>
+  </si>
+  <si>
+    <t>0.00614</t>
+  </si>
+  <si>
+    <t>0.00189</t>
+  </si>
+  <si>
+    <t>0.00116</t>
+  </si>
+  <si>
+    <t>0.00240</t>
+  </si>
+  <si>
+    <t>0.00379</t>
+  </si>
+  <si>
+    <t>0.00154</t>
+  </si>
+  <si>
+    <t>0.00313</t>
+  </si>
+  <si>
+    <t>0.00537</t>
+  </si>
+  <si>
+    <t>0.00724</t>
+  </si>
+  <si>
+    <t>0.00857</t>
+  </si>
+  <si>
+    <t>0.00097</t>
+  </si>
+  <si>
+    <t>0.00257</t>
+  </si>
+  <si>
+    <t>0.02476</t>
+  </si>
+  <si>
+    <t>0.05089</t>
+  </si>
+  <si>
+    <t>0.00263</t>
+  </si>
+  <si>
+    <t>0.00147</t>
+  </si>
+  <si>
+    <t>0.00303</t>
+  </si>
+  <si>
+    <t>0.00327</t>
+  </si>
+  <si>
+    <t>0.00215</t>
+  </si>
+  <si>
+    <t>0.00145</t>
+  </si>
+  <si>
+    <t>0.00550</t>
+  </si>
+  <si>
+    <t>0.00647</t>
+  </si>
+  <si>
+    <t>0.03039</t>
+  </si>
+  <si>
+    <t>0.00086</t>
+  </si>
+  <si>
+    <t>0.00151</t>
+  </si>
+  <si>
+    <t>0.00094</t>
+  </si>
+  <si>
+    <t>0.02727</t>
+  </si>
+  <si>
+    <t>0.00218</t>
+  </si>
+  <si>
+    <t>0.00083</t>
+  </si>
+  <si>
+    <t>0.00743</t>
+  </si>
+  <si>
+    <t>0.01528</t>
+  </si>
+  <si>
+    <t>0.00053</t>
+  </si>
+  <si>
+    <t>0.00069</t>
+  </si>
+  <si>
+    <t>0.00054</t>
+  </si>
+  <si>
+    <t>0.02169</t>
+  </si>
+  <si>
+    <t>0.00046</t>
+  </si>
+  <si>
+    <t>0.01089</t>
+  </si>
+  <si>
+    <t>0.00062</t>
+  </si>
+  <si>
+    <t>0.00047</t>
+  </si>
+  <si>
+    <t>0.00063</t>
+  </si>
+  <si>
+    <t>0.00039</t>
+  </si>
+  <si>
+    <t>0.00040</t>
+  </si>
+  <si>
+    <t>0.00051</t>
+  </si>
+  <si>
+    <t>0.00041</t>
+  </si>
+  <si>
+    <t>0.00033</t>
+  </si>
+  <si>
+    <t>0.01720</t>
+  </si>
+  <si>
+    <t>0.00030</t>
+  </si>
+  <si>
+    <t>0.51342</t>
+  </si>
+  <si>
+    <t>0.00024</t>
+  </si>
+  <si>
+    <t>0.00025</t>
+  </si>
+  <si>
+    <t>0.01936</t>
+  </si>
+  <si>
+    <t>0.00018</t>
+  </si>
+  <si>
+    <t>0.03826</t>
+  </si>
+  <si>
+    <t>0.00011</t>
+  </si>
+  <si>
+    <t>0.00015</t>
+  </si>
+  <si>
+    <t>0.00013</t>
+  </si>
+  <si>
+    <t>0.00010</t>
+  </si>
+  <si>
+    <t>0.00008</t>
+  </si>
+  <si>
+    <t>0.00009</t>
+  </si>
+  <si>
+    <t>0.00007</t>
+  </si>
+  <si>
+    <t>0.01239</t>
+  </si>
+  <si>
+    <t>0.00452</t>
+  </si>
+  <si>
+    <t>0.00929</t>
+  </si>
+  <si>
+    <t>0.03394</t>
+  </si>
+  <si>
+    <t>0.04427</t>
+  </si>
+  <si>
+    <t>0.05622</t>
+  </si>
+  <si>
+    <t>0.06434</t>
+  </si>
+  <si>
+    <t>0.07585</t>
+  </si>
+  <si>
+    <t>0.08510</t>
+  </si>
+  <si>
+    <t>0.09660</t>
+  </si>
+  <si>
+    <t>0.10625</t>
+  </si>
+  <si>
+    <t>0.11992</t>
+  </si>
+  <si>
+    <t>0.13989</t>
+  </si>
+  <si>
+    <t>0.15276</t>
+  </si>
+  <si>
+    <t>0.17355</t>
+  </si>
+  <si>
+    <t>0.19311</t>
+  </si>
+  <si>
+    <t>0.21459</t>
+  </si>
+  <si>
+    <t>0.23534</t>
+  </si>
+  <si>
+    <t>0.25839</t>
+  </si>
+  <si>
+    <t>0.28231</t>
+  </si>
+  <si>
+    <t>0.30686</t>
+  </si>
+  <si>
+    <t>0.33180</t>
+  </si>
+  <si>
+    <t>0.35684</t>
+  </si>
+  <si>
+    <t>0.38171</t>
+  </si>
+  <si>
+    <t>0.40613</t>
+  </si>
+  <si>
+    <t>0.42983</t>
+  </si>
+  <si>
+    <t>0.45259</t>
+  </si>
+  <si>
+    <t>0.47420</t>
+  </si>
+  <si>
+    <t>0.49451</t>
+  </si>
+  <si>
+    <t>0.53086</t>
+  </si>
+  <si>
+    <t>0.54681</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,10 +685,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,19 +1003,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E1" sqref="E1:N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -738,891 +1023,891 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>3.13E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>2.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>1.8000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>1.2999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>8.0000000000000007E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>9.0000000000000006E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>6.9999999999999994E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>6.9999999999999994E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>8.0000000000000007E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>9.0000000000000006E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>8.0000000000000007E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>8.0000000000000007E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>1.4999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>1.1E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>2.5000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>2.5000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>2.9999999999999997E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>3.8999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>4.0000000000000002E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>4.0999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>3.3E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>3.8999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>4.6999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>4.0000000000000002E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>4.0999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>4.6999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30">
-        <v>4.6000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B31">
-        <v>5.2999999999999998E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32">
-        <v>5.1000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
-        <v>6.2E-4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
-        <v>6.3000000000000003E-4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B35">
-        <v>6.3000000000000003E-4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B36">
-        <v>6.8999999999999997E-4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B37">
-        <v>8.3000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B38">
-        <v>8.5999999999999998E-4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B39">
-        <v>8.3000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B40">
-        <v>9.3999999999999997E-4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B41">
-        <v>9.7000000000000005E-4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B42">
-        <v>1.0499999999999999E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B43">
-        <v>1.16E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B44">
-        <v>1.31E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B45">
-        <v>1.4499999999999999E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B46">
-        <v>1.47E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B47">
-        <v>1.5100000000000001E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B48">
-        <v>1.5399999999999999E-3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B49">
-        <v>1.89E-3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B50">
-        <v>2.15E-3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B51">
-        <v>2.1800000000000001E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B52">
-        <v>2.3999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B53">
-        <v>2.5699999999999998E-3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B54">
-        <v>2.63E-3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B55">
-        <v>3.0300000000000001E-3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B56">
-        <v>3.2699999999999999E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B57">
-        <v>3.5500000000000002E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B58">
-        <v>3.79E-3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B59">
-        <v>4.0899999999999999E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B60">
-        <v>4.5199999999999997E-3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B61">
-        <v>4.6299999999999996E-3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B62">
-        <v>5.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B63">
-        <v>5.3699999999999998E-3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B64">
-        <v>6.1399999999999996E-3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B65">
-        <v>6.4700000000000001E-3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B66">
-        <v>7.2399999999999999E-3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B67">
-        <v>7.43E-3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B68">
-        <v>8.5699999999999995E-3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B69">
-        <v>9.2899999999999996E-3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B70">
-        <v>1.089E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B71">
-        <v>1.0880000000000001E-2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B72">
-        <v>1.239E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B73">
-        <v>1.4290000000000001E-2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B74">
-        <v>1.528E-2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B75">
-        <v>1.72E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B76">
-        <v>1.9359999999999999E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B77">
-        <v>2.1690000000000001E-2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B78">
-        <v>2.4760000000000001E-2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B79">
-        <v>2.7269999999999999E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B80">
-        <v>3.039E-2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B81">
-        <v>3.3939999999999998E-2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B82">
-        <v>3.8260000000000002E-2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B83">
-        <v>4.4269999999999997E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B84">
-        <v>5.0889999999999998E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B85">
-        <v>5.6219999999999999E-2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B86">
-        <v>6.4339999999999994E-2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B87">
-        <v>7.5850000000000001E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B88">
-        <v>8.5099999999999995E-2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B89">
-        <v>9.6600000000000005E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B90">
-        <v>0.10625</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B91">
-        <v>0.11992</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B92">
-        <v>0.13988999999999999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B93">
-        <v>0.15276000000000001</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B94">
-        <v>0.17355000000000001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B95">
-        <v>0.19311</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B96">
-        <v>0.21459</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B97">
-        <v>0.23533999999999999</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B98">
-        <v>0.25839000000000001</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B99">
-        <v>0.28231000000000001</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B100">
-        <v>0.30686000000000002</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B101">
-        <v>0.33179999999999998</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>100</v>
       </c>
-      <c r="B102">
-        <v>0.35683999999999999</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>101</v>
       </c>
-      <c r="B103">
-        <v>0.38170999999999999</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>102</v>
       </c>
-      <c r="B104">
-        <v>0.40612999999999999</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>103</v>
       </c>
-      <c r="B105">
-        <v>0.42982999999999999</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>104</v>
       </c>
-      <c r="B106">
-        <v>0.45258999999999999</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>105</v>
       </c>
-      <c r="B107">
-        <v>0.47420000000000001</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>106</v>
       </c>
-      <c r="B108">
-        <v>0.49451000000000001</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>107</v>
       </c>
-      <c r="B109">
-        <v>0.51341999999999999</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>108</v>
       </c>
-      <c r="B110">
-        <v>0.53086</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>109</v>
       </c>
-      <c r="B111">
-        <v>0.54681000000000002</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>102</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>